<commit_message>
casos de uso web
</commit_message>
<xml_diff>
--- a/documentacion/PL02.-Elementos-y-Trazabilidad.xlsx
+++ b/documentacion/PL02.-Elementos-y-Trazabilidad.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
   <si>
     <t>ID Caso de Uso</t>
   </si>
@@ -157,10 +157,76 @@
     <t>El sistema tendrá una pantalla para gestionar usuarios donde se puede dar de alta ,listar,buscar , modificar y borrar usuarios</t>
   </si>
   <si>
-    <t>borrar usuario</t>
-  </si>
-  <si>
-    <t>editar Usuario</t>
+    <t>Alta servicio</t>
+  </si>
+  <si>
+    <t>Listar Servicios</t>
+  </si>
+  <si>
+    <t>Buscar Servicios</t>
+  </si>
+  <si>
+    <t>editar Servicios</t>
+  </si>
+  <si>
+    <t>borrar servicios</t>
+  </si>
+  <si>
+    <t>Editar usuarios</t>
+  </si>
+  <si>
+    <t>borrar usuarios</t>
+  </si>
+  <si>
+    <t>Alta evento</t>
+  </si>
+  <si>
+    <t>Listar eventos</t>
+  </si>
+  <si>
+    <t>Buscar eventos</t>
+  </si>
+  <si>
+    <t>borrar eventos</t>
+  </si>
+  <si>
+    <t>editar eventos</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>estadisticas</t>
+  </si>
+  <si>
+    <t>prototipo usuarios</t>
+  </si>
+  <si>
+    <t>5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>prototipo login</t>
+  </si>
+  <si>
+    <t>prototipo eventos</t>
+  </si>
+  <si>
+    <t>prototipo servicios</t>
+  </si>
+  <si>
+    <t>prototipo web publica</t>
+  </si>
+  <si>
+    <t>prototipo estadisticas</t>
+  </si>
+  <si>
+    <t>15,16,17,19,19</t>
+  </si>
+  <si>
+    <t>10,11,12,13,14</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
   </si>
 </sst>
 </file>
@@ -572,8 +638,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -708,7 +786,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="35">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -720,6 +798,12 @@
     <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -731,6 +815,12 @@
     <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1009,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1124,9 +1214,15 @@
         <v>1</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
+      <c r="J4" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="22">
+        <v>1</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="N4" s="21"/>
       <c r="O4" s="21"/>
       <c r="P4" s="21"/>
@@ -1151,9 +1247,15 @@
         <v>2</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="J5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="20">
+        <v>2</v>
+      </c>
+      <c r="L5" s="20">
+        <v>4</v>
+      </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
@@ -1178,9 +1280,15 @@
         <v>3</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="J6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="20">
+        <v>3</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -1205,9 +1313,15 @@
         <v>4</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="J7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="20">
+        <v>4</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
@@ -1232,9 +1346,15 @@
         <v>5</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="J8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="20">
+        <v>5</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
@@ -1259,9 +1379,15 @@
         <v>5</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
+      <c r="J9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="20">
+        <v>6</v>
+      </c>
+      <c r="L9" s="20">
+        <v>21</v>
+      </c>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -1304,7 +1430,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G11" s="7">
         <v>8</v>
@@ -1330,8 +1456,8 @@
       <c r="D12" s="7">
         <v>9</v>
       </c>
-      <c r="F12" s="42" t="s">
-        <v>44</v>
+      <c r="F12" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="G12" s="7">
         <v>9</v>
@@ -1346,6 +1472,138 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="F13" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="7">
+        <v>10</v>
+      </c>
+      <c r="H13" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="F14" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="7">
+        <v>11</v>
+      </c>
+      <c r="H14" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="F15" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="7">
+        <v>12</v>
+      </c>
+      <c r="H15" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="F16" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="7">
+        <v>13</v>
+      </c>
+      <c r="H16" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8">
+      <c r="F17" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="7">
+        <v>14</v>
+      </c>
+      <c r="H17" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8">
+      <c r="F18" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="7">
+        <v>15</v>
+      </c>
+      <c r="H18" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8">
+      <c r="F19" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="7">
+        <v>16</v>
+      </c>
+      <c r="H19" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8">
+      <c r="F20" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="7">
+        <v>17</v>
+      </c>
+      <c r="H20" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8">
+      <c r="F21" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="7">
+        <v>18</v>
+      </c>
+      <c r="H21" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8">
+      <c r="F22" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="7">
+        <v>19</v>
+      </c>
+      <c r="H22" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8">
+      <c r="F23" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="7">
+        <v>20</v>
+      </c>
+      <c r="H23" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="6:8">
+      <c r="F24" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="7">
+        <v>21</v>
+      </c>
+      <c r="H24" s="7">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
finalizado casos pruebas web
</commit_message>
<xml_diff>
--- a/documentacion/PL02.-Elementos-y-Trazabilidad.xlsx
+++ b/documentacion/PL02.-Elementos-y-Trazabilidad.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
   <si>
     <t>ID Caso de Uso</t>
   </si>
@@ -338,6 +338,15 @@
   </si>
   <si>
     <t>Borrar Servicois</t>
+  </si>
+  <si>
+    <t>Alta eventos</t>
+  </si>
+  <si>
+    <t>listar eventos</t>
+  </si>
+  <si>
+    <t>buscar eventos</t>
   </si>
 </sst>
 </file>
@@ -754,8 +763,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -911,7 +922,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="43">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -932,6 +943,7 @@
     <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -952,6 +964,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1222,7 +1235,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1232,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="K14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1880,9 +1893,15 @@
       <c r="H20" s="7">
         <v>7</v>
       </c>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
+      <c r="N20" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="O20" s="7">
+        <v>17</v>
+      </c>
+      <c r="P20" s="7">
+        <v>7</v>
+      </c>
     </row>
     <row r="21" spans="2:16" ht="44">
       <c r="B21" s="35" t="s">
@@ -1903,9 +1922,15 @@
       <c r="H21" s="7">
         <v>7</v>
       </c>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
+      <c r="N21" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="O21" s="7">
+        <v>18</v>
+      </c>
+      <c r="P21" s="7">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="2:16" ht="22">
       <c r="B22" s="35" t="s">
@@ -1926,9 +1951,15 @@
       <c r="H22" s="7">
         <v>7</v>
       </c>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
+      <c r="N22" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="O22" s="7">
+        <v>19</v>
+      </c>
+      <c r="P22" s="7">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="2:16" ht="22">
       <c r="B23" s="35" t="s">
@@ -1949,9 +1980,15 @@
       <c r="H23" s="7">
         <v>8</v>
       </c>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
+      <c r="N23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="O23" s="7">
+        <v>20</v>
+      </c>
+      <c r="P23" s="7">
+        <v>7</v>
+      </c>
     </row>
     <row r="24" spans="2:16" ht="55">
       <c r="B24" s="35" t="s">
@@ -1971,6 +2008,15 @@
       </c>
       <c r="H24" s="7">
         <v>9</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="O24" s="7">
+        <v>21</v>
+      </c>
+      <c r="P24" s="7">
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="22">
@@ -2112,6 +2158,7 @@
     <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
casos de prueba mobile
</commit_message>
<xml_diff>
--- a/documentacion/PL02.-Elementos-y-Trazabilidad.xlsx
+++ b/documentacion/PL02.-Elementos-y-Trazabilidad.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
   <si>
     <t>ID Caso de Uso</t>
   </si>
@@ -241,119 +241,254 @@
     <t>El sistema permitirá ingresar usuarios indistinto de su rol.</t>
   </si>
   <si>
+    <t xml:space="preserve"> El sistema mostrará un listado de servicios vigentes.</t>
+  </si>
+  <si>
+    <t>El sistema permitirá la contratación de los mismos a través de un link de Mercado Pago.</t>
+  </si>
+  <si>
+    <t>El sistema mostrará un listado de eventos vigentes</t>
+  </si>
+  <si>
+    <t>El sistema mostrará un listado de mis mascotas cargadas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El sistema permitirá al usuario crear una mascota para dar en adopción</t>
+  </si>
+  <si>
+    <t>El sistema mostrará un listado de mascotas disponibles en adopción con un botón de contacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El sistema permitirá al usuario filtrar la búsqueda por sexo, tamaño, edad y distancia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema permitirá al usuario a través del botón de contacto mandar un mail al rescatista de la mascota elegida para establecer un contacto
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El sistema tendrá una opción para desloguearse del sistema y luego lo redirigirá a al Login.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Los administradores del sistema web deben poder aprender a gestionar usuarios, eventos y servicios de manera sencilla e intuitiva</t>
+  </si>
+  <si>
+    <t>La aplicación web debe ser compatible con los siguientes exploradores: Internet Explorer, Google Chrome, Safari</t>
+  </si>
+  <si>
+    <t>Las contraseñas se almacenaran en base de datos de forma encriptada</t>
+  </si>
+  <si>
+    <t>El tiempo para iniciar o reiniciar el sistema no debe ser extenso</t>
+  </si>
+  <si>
+    <t>El proceso de desarrollo debe permitir subir cambios al servidor web y deployarlos en producción de forma sencilla para minimizar tiempo de espera de resolución de fallos y de indisponibilidad del servicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Los sistemas tanto mobile como web deben contar con interfaces de usuarios definidas de forma homogénea</t>
+  </si>
+  <si>
+    <t>no funcional</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El sistema mostrara un listado de eventos vigentes </t>
+  </si>
+  <si>
+    <t>Listar eventos vigentes</t>
+  </si>
+  <si>
+    <t>Listar usuario</t>
+  </si>
+  <si>
+    <t>Buscar usuario</t>
+  </si>
+  <si>
+    <t>Borrar usuario</t>
+  </si>
+  <si>
+    <t>editar usuario</t>
+  </si>
+  <si>
+    <t>Buscar servicios</t>
+  </si>
+  <si>
+    <t>Editar servicio</t>
+  </si>
+  <si>
+    <t>Borrar Servicois</t>
+  </si>
+  <si>
+    <t>Alta eventos</t>
+  </si>
+  <si>
+    <t>listar eventos</t>
+  </si>
+  <si>
+    <t>buscar eventos</t>
+  </si>
+  <si>
+    <t>Las altas ,bajas ,modificaciones,listados,buquedas funcionan de la misma manera en usuarios, eventos y servicios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se utilizo la libreria bootsrap para diseñar las interfaces graficas </t>
+  </si>
+  <si>
+    <t>El sistema  debe contar con textos que tengan un lenguaje amigable al usuario evitando el uso de términos técnicos</t>
+  </si>
+  <si>
+    <t>Se utilizo lenguaje natural para los textos de la web y de la app mobile</t>
+  </si>
+  <si>
+    <t>Se utilizo spring security con un password encoder con  el algoritmo bcrypt para encriptar las claves en base de datos</t>
+  </si>
+  <si>
+    <t>Únicamente los usuarios con rol de administrador podrán gestionar  la aplicación</t>
+  </si>
+  <si>
+    <t>Se asignan roles a los usuarios , ADMIN o USER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se utilizo el framework spingboot con una app autoejecutable con tomcat embebido la cual una vez compilada se ejecuta con un simple comando, no hace falta configurar ni deployar la aplicacion en un tomcat aparte, reduciendo los tiempos </t>
+  </si>
+  <si>
+    <t>Se elegio como hosting heroku , y el codigo fuente de la aplicacion web esta en github, para deployar un cambio solo pusheamos del branch local al git de heroku y automaticamente toma los cambios, los compila y deploya la aplicacion</t>
+  </si>
+  <si>
+    <t>Las pantallas tienen uniformidad y cada una tiene una funcionalidad definida</t>
+  </si>
+  <si>
+    <t>UX</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>La aplicacion permitira el acceso de multiples usuarios al mismo tiempo</t>
+  </si>
+  <si>
+    <t>no tiene impacto en el diseño</t>
+  </si>
+  <si>
+    <t>eventos</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>usuario-persona-rol</t>
+  </si>
+  <si>
+    <t>mascota</t>
+  </si>
+  <si>
+    <t>relacional</t>
+  </si>
+  <si>
+    <t>mascota-usuario-coordenadas</t>
+  </si>
+  <si>
+    <t>Servicios</t>
+  </si>
+  <si>
+    <t>servicios-prestador</t>
+  </si>
+  <si>
+    <t>EL usuario se registra en la bbdd como una relacion de herencia entre usuario-persona y como una relacion *-1 con rol</t>
+  </si>
+  <si>
+    <t>las mascotas se registran en bbdd como una relacion 1-* entre mascota ,usuario y 1-* entre mascota y coordenadas</t>
+  </si>
+  <si>
+    <t>Los servicios se guardan como una relacion 1-* entre   prestador y servicios</t>
+  </si>
+  <si>
+    <t>evento</t>
+  </si>
+  <si>
+    <t>los eventos se guardan en la tabla eventos</t>
+  </si>
+  <si>
+    <t>Login con facebook</t>
+  </si>
+  <si>
+    <t>crear usuario</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>login con facebook</t>
+  </si>
+  <si>
+    <r>
+      <t>  El sistema permitirá loguearse con facebook y en caso de no contar con una cuenta ya hecha creara una con rol de usuari</t>
+    </r>
     <r>
       <rPr>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>  El sistema permitirá la creación de cuentas con rol USUARIO a través del servicio de Facebook.</t>
+      <t>o</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> El sistema mostrará un listado de servicios vigentes.</t>
-  </si>
-  <si>
-    <t>El sistema permitirá la contratación de los mismos a través de un link de Mercado Pago.</t>
-  </si>
-  <si>
-    <t>El sistema mostrará un listado de eventos vigentes</t>
-  </si>
-  <si>
-    <t>El sistema mostrará un listado de mis mascotas cargadas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> El sistema permitirá al usuario crear una mascota para dar en adopción</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El sistema permitirá al usuario dar de baja la mascota una vez que ya esté dada en adopción.
+    <t>Listado de servicios</t>
+  </si>
+  <si>
+    <t>Contratar servicio</t>
+  </si>
+  <si>
+    <t>Listado de eventos</t>
+  </si>
+  <si>
+    <t>Listado de mis mascotas</t>
+  </si>
+  <si>
+    <t>Crear mascota</t>
+  </si>
+  <si>
+    <t>Mascota adoptada</t>
+  </si>
+  <si>
+    <t>Listado de mascotas en adopción</t>
+  </si>
+  <si>
+    <t>Filtrar mascotas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema permitirá al usuario dar de baja una   mascota del listado de disponibles una vez que ya esté dada en adopción.
 </t>
   </si>
   <si>
-    <t>El sistema mostrará un listado de mascotas disponibles en adopción con un botón de contacto</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> El sistema permitirá al usuario filtrar la búsqueda por sexo, tamaño, edad y distancia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El sistema permitirá al usuario a través del botón de contacto mandar un mail al rescatista de la mascota elegida para establecer un contacto
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> El sistema tendrá una opción para desloguearse del sistema y luego lo redirigirá a al Login.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Los administradores del sistema web deben poder aprender a gestionar usuarios, eventos y servicios de manera sencilla e intuitiva</t>
-  </si>
-  <si>
-    <t>La aplicación web debe ser compatible con los siguientes exploradores: Internet Explorer, Google Chrome, Safari</t>
-  </si>
-  <si>
-    <t>El sistema mobile debe contar con textos que tengan un lenguaje amigable al usuario evitando el uso de términos técnicos</t>
-  </si>
-  <si>
-    <t>Las contraseñas se almacenaran en base de datos de forma encriptada</t>
-  </si>
-  <si>
-    <t>Únicamente los usuarios con rol de administrador podrán gestionar usuarios de la aplicación</t>
-  </si>
-  <si>
-    <t>El tiempo para iniciar o reiniciar el sistema no debe ser extenso</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> El sistema  web debe contar con un sistema sencillo de deploy en el servidor</t>
-  </si>
-  <si>
-    <t>El proceso de desarrollo debe permitir subir cambios al servidor web y deployarlos en producción de forma sencilla para minimizar tiempo de espera de resolución de fallos y de indisponibilidad del servicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Los sistemas tanto mobile como web deben contar con interfaces de usuarios definidas de forma homogénea</t>
-  </si>
-  <si>
-    <t>no funcional</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> El sistema mostrara un listado de eventos vigentes </t>
-  </si>
-  <si>
-    <t>Listar eventos vigentes</t>
-  </si>
-  <si>
-    <t>Listar usuario</t>
-  </si>
-  <si>
-    <t>Buscar usuario</t>
-  </si>
-  <si>
-    <t>Borrar usuario</t>
-  </si>
-  <si>
-    <t>editar usuario</t>
-  </si>
-  <si>
-    <t>Buscar servicios</t>
-  </si>
-  <si>
-    <t>Editar servicio</t>
-  </si>
-  <si>
-    <t>Borrar Servicois</t>
-  </si>
-  <si>
-    <t>Alta eventos</t>
-  </si>
-  <si>
-    <t>listar eventos</t>
-  </si>
-  <si>
-    <t>buscar eventos</t>
+    <t>Contactar a otro usuario</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Crear usuario</t>
+  </si>
+  <si>
+    <t>usuario logueado</t>
+  </si>
+  <si>
+    <t>contratar servicios</t>
+  </si>
+  <si>
+    <t>crear mascotas</t>
+  </si>
+  <si>
+    <t>adoptar mascotas</t>
+  </si>
+  <si>
+    <t>contactar a otro usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +568,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -763,7 +903,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -807,8 +947,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -891,9 +1043,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -921,8 +1070,12 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="55">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -944,6 +1097,12 @@
     <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -965,6 +1124,12 @@
     <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1243,10 +1408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="K29" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1273,28 +1438,28 @@
   <sheetData>
     <row r="1" spans="1:16" ht="7.5" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:16" s="5" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="39"/>
-      <c r="N2" s="40" t="s">
+      <c r="K2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="N2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="42"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="41"/>
     </row>
     <row r="3" spans="1:16" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="2"/>
@@ -1418,7 +1583,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="B6" s="34" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>27</v>
@@ -1485,7 +1650,7 @@
         <v>64</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="O7" s="7">
         <v>4</v>
@@ -1495,7 +1660,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="33">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="34" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -1534,7 +1699,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="33">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="34" t="s">
         <v>39</v>
       </c>
       <c r="C9" s="21" t="s">
@@ -1563,7 +1728,7 @@
         <v>21</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="O9" s="7">
         <v>6</v>
@@ -1573,7 +1738,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="55">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="34" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="21" t="s">
@@ -1596,7 +1761,7 @@
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
       <c r="N10" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="O10" s="7">
         <v>7</v>
@@ -1606,7 +1771,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="44">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="34" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="21" t="s">
@@ -1629,7 +1794,7 @@
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
       <c r="N11" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="O11" s="7">
         <v>8</v>
@@ -1639,7 +1804,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="33">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="34" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="21" t="s">
@@ -1662,7 +1827,7 @@
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
       <c r="N12" s="7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="O12" s="7">
         <v>9</v>
@@ -1672,7 +1837,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="33">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>69</v>
       </c>
       <c r="C13" s="21" t="s">
@@ -1701,7 +1866,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="22">
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="34" t="s">
         <v>70</v>
       </c>
       <c r="C14" s="21" t="s">
@@ -1729,9 +1894,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="18">
-      <c r="B15" s="36" t="s">
-        <v>71</v>
+    <row r="15" spans="1:16" ht="33">
+      <c r="B15" s="34" t="s">
+        <v>130</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>27</v>
@@ -1759,8 +1924,8 @@
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="B16" s="35" t="s">
-        <v>72</v>
+      <c r="B16" s="34" t="s">
+        <v>71</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>27</v>
@@ -1778,7 +1943,7 @@
         <v>6</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="O16" s="7">
         <v>13</v>
@@ -1788,8 +1953,8 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="22">
-      <c r="B17" s="35" t="s">
-        <v>73</v>
+      <c r="B17" s="34" t="s">
+        <v>72</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>27</v>
@@ -1807,7 +1972,7 @@
         <v>6</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="O17" s="7">
         <v>14</v>
@@ -1817,8 +1982,8 @@
       </c>
     </row>
     <row r="18" spans="2:16">
-      <c r="B18" s="35" t="s">
-        <v>74</v>
+      <c r="B18" s="34" t="s">
+        <v>73</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>27</v>
@@ -1836,7 +2001,7 @@
         <v>7</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O18" s="7">
         <v>15</v>
@@ -1846,8 +2011,8 @@
       </c>
     </row>
     <row r="19" spans="2:16" ht="22">
-      <c r="B19" s="35" t="s">
-        <v>75</v>
+      <c r="B19" s="34" t="s">
+        <v>74</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>27</v>
@@ -1875,8 +2040,8 @@
       </c>
     </row>
     <row r="20" spans="2:16" ht="22">
-      <c r="B20" s="35" t="s">
-        <v>76</v>
+      <c r="B20" s="34" t="s">
+        <v>75</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>27</v>
@@ -1894,7 +2059,7 @@
         <v>7</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="O20" s="7">
         <v>17</v>
@@ -1903,9 +2068,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="44">
-      <c r="B21" s="35" t="s">
-        <v>77</v>
+    <row r="21" spans="2:16" ht="55">
+      <c r="B21" s="34" t="s">
+        <v>139</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>27</v>
@@ -1923,7 +2088,7 @@
         <v>7</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="O21" s="7">
         <v>18</v>
@@ -1933,8 +2098,8 @@
       </c>
     </row>
     <row r="22" spans="2:16" ht="22">
-      <c r="B22" s="35" t="s">
-        <v>78</v>
+      <c r="B22" s="34" t="s">
+        <v>76</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>27</v>
@@ -1952,7 +2117,7 @@
         <v>7</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="O22" s="7">
         <v>19</v>
@@ -1962,8 +2127,8 @@
       </c>
     </row>
     <row r="23" spans="2:16" ht="22">
-      <c r="B23" s="35" t="s">
-        <v>79</v>
+      <c r="B23" s="34" t="s">
+        <v>77</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>27</v>
@@ -1991,8 +2156,8 @@
       </c>
     </row>
     <row r="24" spans="2:16" ht="55">
-      <c r="B24" s="35" t="s">
-        <v>80</v>
+      <c r="B24" s="34" t="s">
+        <v>78</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>27</v>
@@ -2020,8 +2185,8 @@
       </c>
     </row>
     <row r="25" spans="2:16" ht="22">
-      <c r="B25" s="35" t="s">
-        <v>81</v>
+      <c r="B25" s="34" t="s">
+        <v>79</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>27</v>
@@ -2029,126 +2194,363 @@
       <c r="D25" s="7">
         <v>22</v>
       </c>
+      <c r="F25" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" s="7">
+        <v>22</v>
+      </c>
+      <c r="H25" s="7">
+        <v>10</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="O25" s="7">
+        <v>22</v>
+      </c>
+      <c r="P25" s="7">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="2:16" ht="33">
-      <c r="B26" s="35" t="s">
-        <v>82</v>
+      <c r="B26" s="34" t="s">
+        <v>80</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D26" s="7">
         <v>23</v>
       </c>
+      <c r="F26" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" s="7">
+        <v>23</v>
+      </c>
+      <c r="H26" s="7">
+        <v>11</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="O26" s="7">
+        <v>23</v>
+      </c>
+      <c r="P26" s="7">
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="2:16" ht="33">
-      <c r="B27" s="35" t="s">
-        <v>83</v>
+      <c r="B27" s="34" t="s">
+        <v>81</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D27" s="7">
         <v>24</v>
       </c>
+      <c r="F27" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="7">
+        <v>24</v>
+      </c>
+      <c r="H27" s="7">
+        <v>12</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="O27" s="7">
+        <v>24</v>
+      </c>
+      <c r="P27" s="7">
+        <v>12</v>
+      </c>
     </row>
     <row r="28" spans="2:16" ht="33">
-      <c r="B28" s="35" t="s">
-        <v>84</v>
+      <c r="B28" s="34" t="s">
+        <v>101</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D28" s="7">
         <v>25</v>
       </c>
+      <c r="F28" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" s="7">
+        <v>25</v>
+      </c>
+      <c r="H28" s="7">
+        <v>13</v>
+      </c>
+      <c r="N28" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="O28" s="7">
+        <v>25</v>
+      </c>
+      <c r="P28" s="7">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="2:16" ht="22">
-      <c r="B29" s="35" t="s">
-        <v>85</v>
+      <c r="B29" s="34" t="s">
+        <v>82</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D29" s="7">
         <v>26</v>
       </c>
+      <c r="F29" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="G29" s="7">
+        <v>26</v>
+      </c>
+      <c r="H29" s="7">
+        <v>14</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="O29" s="7">
+        <v>26</v>
+      </c>
+      <c r="P29" s="7">
+        <v>13</v>
+      </c>
     </row>
     <row r="30" spans="2:16" ht="22">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>86</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>91</v>
       </c>
       <c r="D30" s="7">
         <v>27</v>
       </c>
+      <c r="F30" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="G30" s="7">
+        <v>27</v>
+      </c>
+      <c r="H30" s="7">
+        <v>15</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="O30" s="7">
+        <v>27</v>
+      </c>
+      <c r="P30" s="7">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="2:16" ht="22">
-      <c r="B31" s="35" t="s">
-        <v>87</v>
+      <c r="B31" s="34" t="s">
+        <v>83</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D31" s="7">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" ht="22">
-      <c r="B32" s="35" t="s">
-        <v>88</v>
+      <c r="F31" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="G31" s="7">
+        <v>28</v>
+      </c>
+      <c r="H31" s="7">
+        <v>16</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O31" s="7">
+        <v>28</v>
+      </c>
+      <c r="P31" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="44">
+      <c r="B32" s="34" t="s">
+        <v>84</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D32" s="7">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" ht="44">
-      <c r="B33" s="35" t="s">
-        <v>89</v>
+      <c r="F32" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="G32" s="7">
+        <v>29</v>
+      </c>
+      <c r="H32" s="7">
+        <v>17</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="O32" s="7">
+        <v>29</v>
+      </c>
+      <c r="P32" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" ht="33">
+      <c r="B33" s="34" t="s">
+        <v>85</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D33" s="7">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" ht="33">
-      <c r="B34" s="35" t="s">
-        <v>90</v>
+      <c r="F33" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G33" s="7">
+        <v>30</v>
+      </c>
+      <c r="H33" s="7">
+        <v>18</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="O33" s="7">
+        <v>30</v>
+      </c>
+      <c r="P33" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" ht="22">
+      <c r="B34" s="34" t="s">
+        <v>111</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D34" s="7">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="2:4">
+      <c r="F34" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="7">
+        <v>31</v>
+      </c>
+      <c r="H34" s="7">
+        <v>19</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="O34" s="7">
+        <v>31</v>
+      </c>
+      <c r="P34" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16">
       <c r="B35" s="35"/>
-    </row>
-    <row r="36" spans="2:4">
+      <c r="F35" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="G35" s="7">
+        <v>34</v>
+      </c>
+      <c r="H35" s="7">
+        <v>20</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="O35" s="7">
+        <v>32</v>
+      </c>
+      <c r="P35" s="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16">
       <c r="B36" s="35"/>
-    </row>
-    <row r="37" spans="2:4">
+      <c r="F36" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="G36" s="7">
+        <v>35</v>
+      </c>
+      <c r="H36" s="7">
+        <v>21</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="O36" s="7">
+        <v>33</v>
+      </c>
+      <c r="P36" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16">
       <c r="B37" s="35"/>
-    </row>
-    <row r="38" spans="2:4">
+      <c r="F37" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="G37" s="7">
+        <v>36</v>
+      </c>
+      <c r="H37" s="7">
+        <v>22</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="O37" s="7">
+        <v>34</v>
+      </c>
+      <c r="P37" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16">
       <c r="B38" s="35"/>
-    </row>
-    <row r="39" spans="2:4">
+      <c r="N38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O38" s="7">
+        <v>35</v>
+      </c>
+      <c r="P38" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16">
       <c r="B39" s="35"/>
-    </row>
-    <row r="40" spans="2:4">
-      <c r="B40" s="35"/>
-    </row>
-    <row r="41" spans="2:4">
-      <c r="B41" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2172,7 +2574,7 @@
   <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2192,23 +2594,23 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1"/>
     <row r="2" spans="2:12" s="18" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="44"/>
+      <c r="H2" s="43"/>
       <c r="I2"/>
-      <c r="J2" s="43" t="s">
+      <c r="J2" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="45"/>
-      <c r="L2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="43"/>
     </row>
     <row r="3" spans="2:12" ht="36.75" customHeight="1">
       <c r="B3" s="16" t="s">
@@ -2240,104 +2642,226 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
-      <c r="B4" s="8"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="9"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="9"/>
-    </row>
-    <row r="5" spans="2:12">
-      <c r="B5" s="8"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="9"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="2:12">
-      <c r="B6" s="8"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="9"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="2:12">
-      <c r="B7" s="8"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="9"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="9"/>
+    <row r="4" spans="2:12" ht="23">
+      <c r="B4" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="7">
+        <v>23</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1</v>
+      </c>
+      <c r="L4" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="23">
+      <c r="B5" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="7">
+        <v>24</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K5" s="7">
+        <v>2</v>
+      </c>
+      <c r="L5" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="23">
+      <c r="B6" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="7">
+        <v>25</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" s="7">
+        <v>3</v>
+      </c>
+      <c r="L6" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="23">
+      <c r="B7" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="7">
+        <v>26</v>
+      </c>
+      <c r="H7" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K7" s="7">
+        <v>4</v>
+      </c>
+      <c r="L7" s="9">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="8"/>
       <c r="C8" s="30"/>
       <c r="D8" s="7"/>
       <c r="E8" s="9"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="2:12">
+      <c r="G8" s="7">
+        <v>27</v>
+      </c>
+      <c r="H8" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K8" s="7">
+        <v>5</v>
+      </c>
+      <c r="L8" s="9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="34">
       <c r="B9" s="8"/>
       <c r="C9" s="30"/>
       <c r="D9" s="7"/>
       <c r="E9" s="9"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="9"/>
-    </row>
-    <row r="10" spans="2:12">
+      <c r="G9" s="7">
+        <v>28</v>
+      </c>
+      <c r="H9" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K9" s="7">
+        <v>6</v>
+      </c>
+      <c r="L9" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="34">
       <c r="B10" s="8"/>
       <c r="C10" s="30"/>
       <c r="D10" s="7"/>
       <c r="E10" s="9"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="9"/>
+      <c r="G10" s="7">
+        <v>29</v>
+      </c>
+      <c r="H10" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="7">
+        <v>7</v>
+      </c>
+      <c r="L10" s="9">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="2:12">
       <c r="B11" s="8"/>
       <c r="C11" s="30"/>
       <c r="D11" s="7"/>
       <c r="E11" s="9"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="9"/>
+      <c r="G11" s="7">
+        <v>30</v>
+      </c>
+      <c r="H11" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K11" s="7">
+        <v>8</v>
+      </c>
+      <c r="L11" s="9">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="2:12">
       <c r="B12" s="8"/>
       <c r="C12" s="30"/>
       <c r="D12" s="7"/>
       <c r="E12" s="9"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="9"/>
+      <c r="G12" s="7">
+        <v>31</v>
+      </c>
+      <c r="H12" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K12" s="7">
+        <v>9</v>
+      </c>
+      <c r="L12" s="9">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="8"/>

</xml_diff>

<commit_message>
todos los doc terminados
</commit_message>
<xml_diff>
--- a/documentacion/PL02.-Elementos-y-Trazabilidad.xlsx
+++ b/documentacion/PL02.-Elementos-y-Trazabilidad.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="159">
   <si>
     <t>ID Caso de Uso</t>
   </si>
@@ -482,6 +482,39 @@
   </si>
   <si>
     <t>contactar a otro usuario</t>
+  </si>
+  <si>
+    <t>Prototipo Login</t>
+  </si>
+  <si>
+    <t>prototipo Mi cuenta</t>
+  </si>
+  <si>
+    <t>prototipo agregar mascota</t>
+  </si>
+  <si>
+    <t>prototipo buscar</t>
+  </si>
+  <si>
+    <t>prototipo evento</t>
+  </si>
+  <si>
+    <t>prototipo filtros</t>
+  </si>
+  <si>
+    <t>prototipo mis mascotas</t>
+  </si>
+  <si>
+    <t>prototipo nueva cuenta</t>
+  </si>
+  <si>
+    <t>11,12</t>
+  </si>
+  <si>
+    <t>13,14</t>
+  </si>
+  <si>
+    <t>16,18</t>
   </si>
 </sst>
 </file>
@@ -1410,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1757,9 +1790,15 @@
         <v>5</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
+      <c r="J10" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="K10" s="20">
+        <v>7</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>156</v>
+      </c>
       <c r="N10" s="7" t="s">
         <v>90</v>
       </c>
@@ -1790,9 +1829,15 @@
         <v>5</v>
       </c>
       <c r="I11" s="4"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
+      <c r="J11" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="K11" s="20">
+        <v>8</v>
+      </c>
+      <c r="L11" s="20">
+        <v>22</v>
+      </c>
       <c r="N11" s="7" t="s">
         <v>91</v>
       </c>
@@ -1823,9 +1868,15 @@
         <v>5</v>
       </c>
       <c r="I12" s="4"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+      <c r="J12" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="K12" s="20">
+        <v>9</v>
+      </c>
+      <c r="L12" s="20">
+        <v>17</v>
+      </c>
       <c r="N12" s="7" t="s">
         <v>92</v>
       </c>
@@ -1855,6 +1906,15 @@
       <c r="H13" s="7">
         <v>6</v>
       </c>
+      <c r="J13" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="K13" s="20">
+        <v>10</v>
+      </c>
+      <c r="L13" s="20">
+        <v>19</v>
+      </c>
       <c r="N13" s="7" t="s">
         <v>54</v>
       </c>
@@ -1884,6 +1944,15 @@
       <c r="H14" s="7">
         <v>6</v>
       </c>
+      <c r="J14" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14" s="20">
+        <v>11</v>
+      </c>
+      <c r="L14" s="20">
+        <v>15</v>
+      </c>
       <c r="N14" s="7" t="s">
         <v>42</v>
       </c>
@@ -1913,6 +1982,15 @@
       <c r="H15" s="7">
         <v>6</v>
       </c>
+      <c r="J15" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="K15" s="20">
+        <v>12</v>
+      </c>
+      <c r="L15" s="20">
+        <v>20</v>
+      </c>
       <c r="N15" s="7" t="s">
         <v>43</v>
       </c>
@@ -1942,6 +2020,15 @@
       <c r="H16" s="7">
         <v>6</v>
       </c>
+      <c r="J16" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="K16" s="20">
+        <v>13</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>158</v>
+      </c>
       <c r="N16" s="7" t="s">
         <v>93</v>
       </c>
@@ -1971,6 +2058,15 @@
       <c r="H17" s="7">
         <v>6</v>
       </c>
+      <c r="J17" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="K17" s="20">
+        <v>14</v>
+      </c>
+      <c r="L17" s="20">
+        <v>10</v>
+      </c>
       <c r="N17" s="7" t="s">
         <v>94</v>
       </c>
@@ -1999,6 +2095,15 @@
       </c>
       <c r="H18" s="7">
         <v>7</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18" s="20">
+        <v>15</v>
+      </c>
+      <c r="L18" s="20" t="s">
+        <v>157</v>
       </c>
       <c r="N18" s="7" t="s">
         <v>95</v>

</xml_diff>